<commit_message>
api call between services
</commit_message>
<xml_diff>
--- a/student-ms-upload/uploads/Data.xlsx
+++ b/student-ms-upload/uploads/Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -390,7 +390,7 @@
   <dimension ref="A40:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59:B60"/>
+      <selection activeCell="O57" sqref="O57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,7 +456,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s">
         <v>9</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
@@ -512,7 +512,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B48" t="s">
         <v>8</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
@@ -540,7 +540,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B50" t="s">
         <v>7</v>
@@ -553,116 +553,36 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>31</v>
-      </c>
-      <c r="B51" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="4">
-        <v>33847</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>41</v>
-      </c>
-      <c r="B52" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" s="4">
-        <v>33450</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>345</v>
-      </c>
-      <c r="B53" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="4">
-        <v>33816</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C53" s="4"/>
+      <c r="D53" s="1"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>656</v>
-      </c>
-      <c r="B54" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="4">
-        <v>33847</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C54" s="4"/>
+      <c r="D54" s="2"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <v>876</v>
-      </c>
-      <c r="B55" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" s="4">
-        <v>33450</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C55" s="4"/>
+      <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <v>43</v>
-      </c>
-      <c r="B56" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="4">
-        <v>33816</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C56" s="4"/>
+      <c r="D56" s="1"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <v>34</v>
-      </c>
-      <c r="B57" t="s">
-        <v>8</v>
-      </c>
-      <c r="C57" s="4">
-        <v>33847</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C57" s="4"/>
+      <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <v>54</v>
-      </c>
-      <c r="B58" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" s="4">
-        <v>33450</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C58" s="4"/>
+      <c r="D58" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -676,16 +596,8 @@
     <hyperlink ref="D48" r:id="rId8"/>
     <hyperlink ref="D49" r:id="rId9"/>
     <hyperlink ref="D50" r:id="rId10"/>
-    <hyperlink ref="D51" r:id="rId11"/>
-    <hyperlink ref="D52" r:id="rId12"/>
-    <hyperlink ref="D53" r:id="rId13"/>
-    <hyperlink ref="D54" r:id="rId14"/>
-    <hyperlink ref="D55" r:id="rId15"/>
-    <hyperlink ref="D56" r:id="rId16"/>
-    <hyperlink ref="D57" r:id="rId17"/>
-    <hyperlink ref="D58" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>